<commit_message>
Correções pontuais na documentação, planilha de risco e product backlog, adição das imagens na pasta correta, adição da imagem de planilha de risco no Excel, adição do grafico de Burndown no excel
</commit_message>
<xml_diff>
--- a/Tecnologia da informação/LotusTech_Planilha de Risco.xlsx
+++ b/Tecnologia da informação/LotusTech_Planilha de Risco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Documentos\LotusTech\Tecnologia da informação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7AA3E82-6330-440B-A97F-06D3BA4ABDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68BF31C-2BA0-4C74-A626-C8FFCE5AB338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FCD81D41-C76D-4FFD-8188-7737F75CEF18}"/>
   </bookViews>
@@ -112,36 +112,21 @@
     <t>Dificuldade em encontrar conteúdo relevante e de qualidade</t>
   </si>
   <si>
-    <t>Ir em eventos sobre saúde mental, conversar com profissionais da aréa, parcerias com instrutores de meditação</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quebra de segurança de dados dos usuários </t>
   </si>
   <si>
-    <t>Criptográfar dados sensíveis</t>
-  </si>
-  <si>
-    <t>A cada backup feito fazer a recuperção dos dados logo após a conclusão para se certificar que os dados não foram corrompidos</t>
-  </si>
-  <si>
     <t>Baixa participação dos usuários no recurso de progresso de bem-estar</t>
   </si>
   <si>
     <t>Mtigar</t>
   </si>
   <si>
-    <t>incorporar a ferramenta de forma que incentive o usuário aderir ao seu coditiano por meio do seu nívelamento na solução</t>
-  </si>
-  <si>
     <t>Mudança na lei geral da proteção de dados (LGPD)</t>
   </si>
   <si>
     <t>Manter-se informado com atualizações e ajustar o projeto conforme necessário</t>
   </si>
   <si>
-    <t>Mudança excessiva nos requesitos</t>
-  </si>
-  <si>
     <t>Implementar práticas de gerenciamento de mudanças rigorosas, documentar claramente requisitos</t>
   </si>
   <si>
@@ -154,22 +139,37 @@
     <t>Falta de versionamento do Projeto</t>
   </si>
   <si>
-    <t xml:space="preserve">Introduzir essa prática ao codiano para se tornar um hábito </t>
-  </si>
-  <si>
     <t>Problema com a gestão de tempo</t>
   </si>
   <si>
-    <t>Aderir a ferramenta de gestão e cronograma de estudo ao codiano para se organizar separando o tempo correto para concluir todos os requesitos no prazo</t>
-  </si>
-  <si>
-    <t>Dificuldade em fazaer os slides de apresntação</t>
-  </si>
-  <si>
-    <t>A cada etapa concluida da projeto fazer um slide para que a apresentação ande paralelamente ao projeto</t>
-  </si>
-  <si>
     <t>Backup de dados corrompido</t>
+  </si>
+  <si>
+    <t>Dificuldade em fazer os slides de apresentação</t>
+  </si>
+  <si>
+    <t>Aderir a ferramenta de gestão e cronograma de estudo ao cotidiano para se organizar separando o tempo correto para concluir todos os requesitos no prazo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduzir essa prática ao cotidiano para se tornar um hábito </t>
+  </si>
+  <si>
+    <t>Mudança excessiva nos requisitos</t>
+  </si>
+  <si>
+    <t>A cada backup feito fazer a recuperação dos dados logo após a conclusão para se certificar que os dados não foram corrompidos</t>
+  </si>
+  <si>
+    <t>incorporar a ferramenta de forma que incentive o usuário aderir ao seu cotidiano por meio do seu nívelamento na solução</t>
+  </si>
+  <si>
+    <t>Criptografar dados sensíveis</t>
+  </si>
+  <si>
+    <t>Ir em eventos sobre saúde mental, conversar com profissionais da área, parcerias com instrutores de meditação</t>
+  </si>
+  <si>
+    <t>A cada etapa concluida do projeto fazer um slide para que a apresentação ande paralelamente ao projeto</t>
   </si>
 </sst>
 </file>
@@ -252,14 +252,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -268,25 +280,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -661,13 +654,13 @@
   <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -676,7 +669,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6"/>
@@ -705,458 +698,523 @@
       <c r="X1" s="6"/>
       <c r="Y1" s="6"/>
     </row>
-    <row r="2" spans="1:25" s="7" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+    <row r="2" spans="1:25" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="13">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4">
         <v>1</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8">
-        <v>2</v>
-      </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8">
-        <v>2</v>
-      </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5">
+        <v>2</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5">
+        <v>2</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="13" t="s">
+      <c r="M2" s="5"/>
+      <c r="N2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="V2" s="8">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="V2" s="5">
         <v>1</v>
       </c>
-      <c r="W2" s="8"/>
-      <c r="X2" s="9" t="s">
+      <c r="W2" s="5"/>
+      <c r="X2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="9"/>
+      <c r="Y2" s="7"/>
     </row>
     <row r="3" spans="1:25" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="13">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5">
         <v>3</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8">
+      <c r="I3" s="5"/>
+      <c r="J3" s="5">
         <v>3</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="13" t="s">
+      <c r="M3" s="5"/>
+      <c r="N3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="V3" s="2">
-        <v>2</v>
-      </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="4" t="s">
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="V3" s="5">
+        <v>2</v>
+      </c>
+      <c r="W3" s="5"/>
+      <c r="X3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" s="4"/>
+      <c r="Y3" s="8"/>
     </row>
     <row r="4" spans="1:25" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="13">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8">
-        <v>2</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8">
-        <v>2</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5">
+        <v>2</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="V4" s="2">
+      <c r="M4" s="5"/>
+      <c r="N4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="V4" s="5">
         <v>3</v>
       </c>
-      <c r="W4" s="2"/>
-      <c r="X4" s="5" t="s">
+      <c r="W4" s="5"/>
+      <c r="X4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Y4" s="5"/>
+      <c r="Y4" s="9"/>
     </row>
     <row r="5" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="13">
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5">
         <v>3</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
         <v>3</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="V5" s="2" t="s">
+      <c r="M5" s="5"/>
+      <c r="N5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="V5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W5" s="2"/>
-      <c r="X5" s="3" t="s">
+      <c r="W5" s="5"/>
+      <c r="X5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" s="2"/>
+      <c r="Y5" s="5"/>
     </row>
     <row r="6" spans="1:25" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="13">
-        <v>2</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8">
-        <v>2</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8">
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5">
         <v>4</v>
       </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="V6" s="2" t="s">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="V6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="W6" s="2"/>
-      <c r="X6" s="3" t="s">
+      <c r="W6" s="5"/>
+      <c r="X6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y6" s="2"/>
+      <c r="Y6" s="5"/>
     </row>
     <row r="7" spans="1:25" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="13">
-        <v>2</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8">
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
         <v>3</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5">
         <v>6</v>
       </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="V7" s="3" t="s">
+      <c r="M7" s="5"/>
+      <c r="N7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="V7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="W7" s="2"/>
-      <c r="X7" s="3" t="s">
+      <c r="W7" s="5"/>
+      <c r="X7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Y7" s="2"/>
+      <c r="Y7" s="5"/>
     </row>
     <row r="8" spans="1:25" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="13">
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8">
-        <v>2</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8">
-        <v>2</v>
-      </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5">
+        <v>2</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="1:25" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="13">
-        <v>2</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8">
-        <v>2</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8">
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4">
+        <v>2</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5">
+        <v>2</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5">
         <v>4</v>
       </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8" t="s">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="1:25" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="13">
-        <v>2</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8">
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5">
         <v>3</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5">
         <v>6</v>
       </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8" t="s">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="1:25" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5">
+        <v>2</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5">
+        <v>2</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="13">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8">
-        <v>2</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8">
-        <v>2</v>
-      </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" s="8"/>
-      <c r="N11" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="1:25" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="13">
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4">
         <v>3</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5">
         <v>3</v>
       </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8">
+      <c r="I12" s="5"/>
+      <c r="J12" s="5">
         <v>9</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M12" s="8"/>
-      <c r="N12" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="1:25" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="13">
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
         <v>1</v>
       </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5">
         <v>1</v>
       </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8" t="s">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="8"/>
-      <c r="N13" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
     </row>
     <row r="16" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:Q10"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:G13"/>
@@ -1173,76 +1231,11 @@
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>